<commit_message>
Add another sheet for range selection.
</commit_message>
<xml_diff>
--- a/test/xlsx/view/cursor-per-sheet.xlsx
+++ b/test/xlsx/view/cursor-per-sheet.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17927"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,21 +9,28 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19680" windowHeight="8760"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19680" windowHeight="8760" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="3">
   <si>
     <t>cursor</t>
+  </si>
+  <si>
+    <t>top-left</t>
+  </si>
+  <si>
+    <t>bottom-right</t>
   </si>
 </sst>
 </file>
@@ -165,7 +172,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="34">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -348,6 +355,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -512,9 +525,10 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -872,7 +886,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
@@ -912,7 +926,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
@@ -926,4 +940,43 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="C5:E8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5:E8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="5" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C5" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+    </row>
+    <row r="6" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+    </row>
+    <row r="7" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+    </row>
+    <row r="8" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>